<commit_message>
phân tích 11 bảng csdl
</commit_message>
<xml_diff>
--- a/DATABASE/phantichcsdl.xlsx
+++ b/DATABASE/phantichcsdl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5D27FC-F898-4632-9A14-BD0E4C922377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E219C092-FB6E-48C0-B5F3-33E5CB7BB497}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="88">
   <si>
     <t>STT</t>
   </si>
@@ -182,17 +182,119 @@
   </si>
   <si>
     <t>Varchar(100)</t>
+  </si>
+  <si>
+    <t>CTHD</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>khóa ngoại bảng DIENTHOAI</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>nvarchar(100)</t>
+  </si>
+  <si>
+    <t>ThanhTien</t>
+  </si>
+  <si>
+    <t>TAIKHOAN</t>
+  </si>
+  <si>
+    <t>char(10)</t>
+  </si>
+  <si>
+    <t>Khóa chính, số điện thoại</t>
+  </si>
+  <si>
+    <t>HoTen</t>
+  </si>
+  <si>
+    <t>TaiKhoan</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>tên đăng nhập</t>
+  </si>
+  <si>
+    <t>MatKhau</t>
+  </si>
+  <si>
+    <t>AnhDaiDien</t>
+  </si>
+  <si>
+    <t>nvarchar(200)</t>
+  </si>
+  <si>
+    <t>LoaiTK</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>1/0 (Admin/User)</t>
+  </si>
+  <si>
+    <t>1/0 (Active/Locked)</t>
+  </si>
+  <si>
+    <t>BINHLUAN</t>
+  </si>
+  <si>
+    <t>Khóa ngoại bảng TAIKHOAN</t>
+  </si>
+  <si>
+    <t>NoiDung</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>1/0 (Duyệt/ Chờ)</t>
+  </si>
+  <si>
+    <t>KHO</t>
+  </si>
+  <si>
+    <t>SLNhap</t>
+  </si>
+  <si>
+    <t>số lượng nhập</t>
+  </si>
+  <si>
+    <t>số lượng tồn</t>
+  </si>
+  <si>
+    <t>1/0 (còn hàng/ hết hàng)</t>
+  </si>
+  <si>
+    <t>SLIDESHOW</t>
+  </si>
+  <si>
+    <t>hình ảnh</t>
+  </si>
+  <si>
+    <t>nvarchar(50)</t>
+  </si>
+  <si>
+    <t>Đang chờ/Đang giao/Giao thành công/ Đã hủy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -200,20 +302,58 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -237,31 +377,109 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,575 +760,1125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI12"/>
+  <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:S4"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.9140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.75" customWidth="1"/>
-    <col min="22" max="22" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.77734375" customWidth="1"/>
+    <col min="32" max="32" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:35" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="M1" s="5" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="M1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="S1" s="5" t="s">
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="S1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="Y1" s="4" t="s">
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="Y1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AE1" s="4" t="s">
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AE1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="H2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="N2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="T2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="1" t="s">
+      <c r="Z2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AE2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AF2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AF2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="3">
-        <v>1</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="3">
-        <v>1</v>
-      </c>
-      <c r="T3" s="2" t="s">
+      <c r="S3" s="2">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="U3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="V3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="W3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Y3" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="2" t="s">
+      <c r="Y3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AB3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AC3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AE3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AE3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AG3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AH3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AI3" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="3">
-        <v>2</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="S4" s="3">
-        <v>2</v>
-      </c>
-      <c r="T4" s="2" t="s">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="S4" s="2">
+        <v>2</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="U4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="Y4" s="3">
-        <v>2</v>
-      </c>
-      <c r="Z4" s="2" t="s">
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="Y4" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AA4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AE4" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AE4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AG4" s="2" t="s">
+      <c r="AG4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="G5" s="3">
-        <v>3</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="M5" s="3">
-        <v>3</v>
-      </c>
-      <c r="N5" s="2" t="s">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="M5" s="2">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="Y5" s="3">
-        <v>3</v>
-      </c>
-      <c r="Z5" s="2" t="s">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="Y5" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AB5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AC5" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="M6" s="3">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="M6" s="2">
         <v>4</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="Y6" s="3">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="Y6" s="2">
         <v>4</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="Z6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AA6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AB6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AC6" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="G7" s="3">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="M7" s="3">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="M7" s="2">
         <v>5</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="Y7" s="3">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="Y7" s="2">
         <v>5</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="Z7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="G8" s="3">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="G8" s="2">
         <v>6</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="M8" s="3">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="M8" s="2">
         <v>6</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="N8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="Y8" s="16">
+        <v>6</v>
+      </c>
+      <c r="Z8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA8" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>7</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="18"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>8</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="G11" s="3">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:35" ht="13.95" x14ac:dyDescent="0.3">
+      <c r="G11" s="2">
         <v>9</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="G12" s="3">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:35" ht="13.95" x14ac:dyDescent="0.3">
+      <c r="G12" s="2">
         <v>10</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="16" spans="1:35" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="G16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="12"/>
+      <c r="M16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="12"/>
+      <c r="S16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="12"/>
+      <c r="Y16" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="12"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S18" s="1">
+        <v>1</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB18" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="M19" s="1">
+        <v>2</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" s="1">
+        <v>2</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" s="1">
+        <v>3</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="1">
+        <v>3</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="S20" s="1">
+        <v>3</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y20" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21" s="1">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="M21" s="1">
+        <v>4</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="S21" s="1">
+        <v>4</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V21" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="G22" s="1">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="M22" s="1">
+        <v>5</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="S22" s="1">
+        <v>5</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="G23" s="1">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G24" s="1">
+        <v>7</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G25" s="1">
+        <v>8</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="G26" s="1">
+        <v>9</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="S16:W16"/>
+    <mergeCell ref="Y16:AC16"/>
     <mergeCell ref="AE1:AI1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>

</xml_diff>

<commit_message>
mô hình class diagram
</commit_message>
<xml_diff>
--- a/DATABASE/phantichcsdl.xlsx
+++ b/DATABASE/phantichcsdl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA48E75A-4FB8-4260-8598-77A7B87A6BE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1043E2FD-2B8F-4896-A6B8-3A386CCA31B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="88">
   <si>
     <t>STT</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>Nvarchar(200)</t>
-  </si>
-  <si>
-    <t>Varchar(200)</t>
   </si>
   <si>
     <t>Varchar(10)</t>
@@ -459,7 +456,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -471,14 +476,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,7 +759,7 @@
   <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +781,7 @@
     <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="38.88671875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="8.77734375" customWidth="1"/>
@@ -795,48 +792,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="G1" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="M1" s="10" t="s">
+      <c r="A1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="G1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="S1" s="10" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="M1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="S1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="Y1" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AE1" s="10" t="s">
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="Y1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AE1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -950,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>6</v>
@@ -980,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>6</v>
@@ -989,13 +986,13 @@
         <v>12</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Y3" s="2">
         <v>1</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>6</v>
@@ -1047,7 +1044,7 @@
         <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M4" s="2">
         <v>2</v>
@@ -1078,7 +1075,7 @@
         <v>30</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
@@ -1089,7 +1086,7 @@
         <v>24</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
@@ -1113,7 +1110,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1132,10 +1129,10 @@
         <v>3</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
@@ -1174,7 +1171,7 @@
         <v>26</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1191,7 +1188,7 @@
         <v>12</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
@@ -1224,7 +1221,7 @@
         <v>27</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1305,15 +1302,15 @@
       <c r="Y9" s="2">
         <v>7</v>
       </c>
-      <c r="Z9" s="16" t="s">
+      <c r="Z9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AA9" s="16" t="s">
+      <c r="AA9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
@@ -1334,10 +1331,10 @@
         <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1356,41 +1353,41 @@
       <c r="K12" s="1"/>
     </row>
     <row r="16" spans="1:35" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="G16" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="13"/>
-      <c r="M16" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="13"/>
-      <c r="S16" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="13"/>
-      <c r="Y16" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="13"/>
+      <c r="A16" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="G16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="17"/>
+      <c r="M16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="17"/>
+      <c r="S16" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="17"/>
+      <c r="Y16" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="17"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -1474,10 +1471,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>7</v>
@@ -1492,13 +1489,13 @@
         <v>26</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>7</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M18" s="1">
         <v>1</v>
@@ -1507,28 +1504,28 @@
         <v>26</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P18" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S18" s="1">
         <v>1</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V18" s="9" t="s">
         <v>12</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Y18" s="1">
         <v>1</v>
@@ -1537,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB18" s="8" t="s">
         <v>7</v>
@@ -1551,25 +1548,25 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G19" s="1">
         <v>2</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1577,44 +1574,44 @@
         <v>2</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S19" s="1">
         <v>2</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Y19" s="1">
         <v>2</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB19" s="9" t="s">
         <v>12</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
@@ -1622,10 +1619,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1633,23 +1630,23 @@
         <v>3</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M20" s="1">
         <v>3</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -1660,11 +1657,11 @@
         <v>21</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V20" s="1"/>
       <c r="W20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y20" s="5">
         <v>3</v>
@@ -1673,11 +1670,11 @@
         <v>15</v>
       </c>
       <c r="AA20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AB20" s="5"/>
       <c r="AC20" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
@@ -1688,7 +1685,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1696,10 +1693,10 @@
         <v>4</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1710,7 +1707,7 @@
         <v>30</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -1721,7 +1718,7 @@
         <v>11</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V21" s="9" t="s">
         <v>12</v>
@@ -1743,7 +1740,7 @@
         <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1751,10 +1748,10 @@
         <v>5</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1765,11 +1762,11 @@
         <v>22</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P22" s="5"/>
       <c r="Q22" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S22" s="1">
         <v>5</v>
@@ -1778,11 +1775,11 @@
         <v>22</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V22" s="1"/>
       <c r="W22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
@@ -1795,10 +1792,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1809,7 +1806,7 @@
         <v>27</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1827,7 +1824,7 @@
         <v>25</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1842,14 +1839,14 @@
         <v>8</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
@@ -1865,11 +1862,11 @@
         <v>22</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
@@ -1879,17 +1876,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="S16:W16"/>
+    <mergeCell ref="Y16:AC16"/>
     <mergeCell ref="AE1:AI1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="S1:W1"/>
     <mergeCell ref="Y1:AC1"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="S16:W16"/>
-    <mergeCell ref="Y16:AC16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>